<commit_message>
added media, TDY number, and treatments
</commit_message>
<xml_diff>
--- a/library/library_2651.xlsx
+++ b/library/library_2651.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A12C7EA-B188-3F40-A347-55363E602D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0229413-909A-E641-A23E-86F038C71A62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="17360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -126,9 +126,6 @@
     <t>AAATGCA</t>
   </si>
   <si>
-    <t>01.09.17</t>
-  </si>
-  <si>
     <t>ACGCGGG</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>H.BROWN</t>
+  </si>
+  <si>
+    <t>01.09.18</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="B3:B45 E2:E45"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -645,7 +645,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -671,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -680,7 +680,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -697,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -723,7 +723,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -732,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -749,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -758,7 +758,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -775,7 +775,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -784,7 +784,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -801,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -810,7 +810,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -827,7 +827,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -836,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -853,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -862,7 +862,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -879,7 +879,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -888,7 +888,7 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>11</v>
@@ -905,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -914,7 +914,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13">
         <v>12</v>
@@ -931,7 +931,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -940,7 +940,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -957,7 +957,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -966,7 +966,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -983,7 +983,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -992,7 +992,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -1009,7 +1009,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -1018,7 +1018,7 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>16</v>
@@ -1035,7 +1035,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -1044,7 +1044,7 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>17</v>
@@ -1061,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -1070,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <v>18</v>
@@ -1087,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1096,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>19</v>
@@ -1113,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1122,7 +1122,7 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21">
         <v>20</v>
@@ -1139,7 +1139,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1148,7 +1148,7 @@
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>21</v>
@@ -1165,7 +1165,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1174,7 +1174,7 @@
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>22</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1200,13 +1200,13 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>11</v>
@@ -1214,10 +1214,10 @@
     </row>
     <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1226,13 +1226,13 @@
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>11</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1252,13 +1252,13 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>11</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1278,13 +1278,13 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27">
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>11</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1304,13 +1304,13 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28">
         <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>11</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1330,13 +1330,13 @@
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29">
         <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>11</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1356,13 +1356,13 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30">
         <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>11</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1382,13 +1382,13 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31">
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>11</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1408,13 +1408,13 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32">
         <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>11</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1434,13 +1434,13 @@
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33">
         <v>32</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>11</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1460,13 +1460,13 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34">
         <v>33</v>
       </c>
       <c r="G34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>11</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1486,13 +1486,13 @@
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F35">
         <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>11</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1512,13 +1512,13 @@
         <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36">
         <v>35</v>
       </c>
       <c r="G36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>11</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1538,13 +1538,13 @@
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37">
         <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>11</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1564,13 +1564,13 @@
         <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38">
         <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>11</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1590,13 +1590,13 @@
         <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F39">
         <v>38</v>
       </c>
       <c r="G39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>11</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1616,13 +1616,13 @@
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F40">
         <v>39</v>
       </c>
       <c r="G40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>11</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1642,13 +1642,13 @@
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F41">
         <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>11</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1668,13 +1668,13 @@
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F42">
         <v>41</v>
       </c>
       <c r="G42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>11</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1694,13 +1694,13 @@
         <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F43">
         <v>42</v>
       </c>
       <c r="G43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>11</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1720,13 +1720,13 @@
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F44">
         <v>43</v>
       </c>
       <c r="G44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>11</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1746,13 +1746,13 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F45">
         <v>44</v>
       </c>
       <c r="G45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>11</v>

</xml_diff>